<commit_message>
Partner 2 tasks added
</commit_message>
<xml_diff>
--- a/workplan.xlsx
+++ b/workplan.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthak\Documents\github_repos\eoo-projects\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A4E0B0-F578-401D-962D-54D47EE5E8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-14145" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,113 +25,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
-  <si>
-    <t xml:space="preserve">Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgroCensus and Crop Yield Detection + Workshop (VU)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional Near-Coastal Satellite Derived Bathymetry using S1/S2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satellite Derived Bathymetry Validation in 4 Countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastlines Enhancement and Cleanup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastlines Rates of Change and Coastal Erosion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMSP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mangroves Enhancement using CoastTrain ML Data with MVI/MFI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACBLUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seagrass Detection (FJ, VU, PNG, SB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PacRIS Migration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCRAFI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LULC and Invasive Species Detection in Identified Areas (FJ, TO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEP Production Cloud Infrastructure, Documentation and Cleanup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional GeoMedian S2/LS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional LULC Methodlogy and Classification (S2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marine Habitat Mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEP Data Exposure and Dissemination Pipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalise dep-tools, Production Creation Pipelines and Workflows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nexus Upgrade and Back-end Enhancements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENVEXP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nexus Metadata Enhancements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add ENVEXP datasets from NIWA and beyond to Nexus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Develop map viewer for ENVEXP data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiji LandCover Mapping Workshop (Training Data Collect Earth)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiji LandCover Mapping Workshop (DEP)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>AgroCensus and Crop Yield Detection + Workshop (VU)</t>
+  </si>
+  <si>
+    <t>DEP</t>
+  </si>
+  <si>
+    <t>Regional Near-Coastal Satellite Derived Bathymetry using S1/S2</t>
+  </si>
+  <si>
+    <t>SDB</t>
+  </si>
+  <si>
+    <t>Satellite Derived Bathymetry Validation in 4 Countries</t>
+  </si>
+  <si>
+    <t>Coastlines Enhancement and Cleanup</t>
+  </si>
+  <si>
+    <t>Coastlines Rates of Change and Coastal Erosion</t>
+  </si>
+  <si>
+    <t>CMSP</t>
+  </si>
+  <si>
+    <t>Mangroves Enhancement using CoastTrain ML Data with MVI/MFI</t>
+  </si>
+  <si>
+    <t>MACBLUE</t>
+  </si>
+  <si>
+    <t>Seagrass Detection (FJ, VU, PNG, SB)</t>
+  </si>
+  <si>
+    <t>PacRIS Migration</t>
+  </si>
+  <si>
+    <t>PCRAFI</t>
+  </si>
+  <si>
+    <t>LULC and Invasive Species Detection in Identified Areas (FJ, TO)</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>DEP Production Cloud Infrastructure, Documentation and Cleanup</t>
+  </si>
+  <si>
+    <t>Regional GeoMedian S2/LS</t>
+  </si>
+  <si>
+    <t>Regional LULC Methodlogy and Classification (S2)</t>
+  </si>
+  <si>
+    <t>Marine Habitat Mapping</t>
+  </si>
+  <si>
+    <t>DEP Data Exposure and Dissemination Pipeline</t>
+  </si>
+  <si>
+    <t>Finalise dep-tools, Production Creation Pipelines and Workflows</t>
+  </si>
+  <si>
+    <t>Nexus Upgrade and Back-end Enhancements</t>
+  </si>
+  <si>
+    <t>ENVEXP</t>
+  </si>
+  <si>
+    <t>Nexus Metadata Enhancements</t>
+  </si>
+  <si>
+    <t>Add ENVEXP datasets from NIWA and beyond to Nexus</t>
+  </si>
+  <si>
+    <t>Develop map viewer for ENVEXP data</t>
+  </si>
+  <si>
+    <t>Fiji LandCover Mapping Workshop (Training Data Collect Earth)</t>
+  </si>
+  <si>
+    <t>Fiji LandCover Mapping Workshop (DEP)</t>
+  </si>
+  <si>
+    <t>Nexus country workshop (Tonga and Vanuatu)</t>
+  </si>
+  <si>
+    <t>PARTNER2</t>
+  </si>
+  <si>
+    <t>Nexus country workshop (Samoa and Cook Islands)</t>
+  </si>
+  <si>
+    <t>Nexus country workshop (Tuvalu and RMI)</t>
+  </si>
+  <si>
+    <t>Link Riskscape and Nexus (incl. workshop in Wellington, NZ)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,22 +154,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -173,123 +177,96 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -297,12 +274,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -331,7 +308,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -352,7 +329,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -403,7 +380,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -421,31 +398,30 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="65.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="65.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="65.71"/>
+    <col min="2" max="3" width="65.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -459,307 +435,358 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="5">
         <v>45261</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="5">
         <v>45412</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="5">
         <v>45323</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="5">
         <v>45473</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="5">
         <v>45444</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="5">
         <v>45656</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="5">
         <v>45231</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="5">
         <v>45442</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="5">
         <v>45442</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="5">
         <v>45641</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="5">
         <v>45292</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="5">
         <v>45381</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="5">
         <v>45352</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="5">
         <v>45534</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="5">
         <v>45231</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="5">
         <v>45290</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="5">
         <v>45413</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="5">
         <v>45503</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="5">
         <v>45292</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="5">
         <v>45350</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="5">
         <v>45627</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="5">
         <v>45321</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="5">
         <v>45536</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="5">
         <v>45626</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="5">
         <v>45474</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="5">
         <v>45656</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="5">
         <v>45323</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="5">
         <v>45412</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="5">
         <v>45292</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="5">
         <v>45350</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="5">
         <v>45261</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="5">
         <v>45381</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="5">
         <v>45231</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="5">
         <v>45381</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="5">
         <v>45323</v>
       </c>
-      <c r="C19" s="6" t="n">
+      <c r="C19" s="5">
         <v>45473</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="5">
         <v>45413</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C20" s="5">
         <v>45656</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="5">
         <v>45313</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="5">
         <v>45317</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="5">
         <v>45341</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="5">
         <v>45345</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>5</v>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="5">
+        <v>45352</v>
+      </c>
+      <c r="C23" s="5">
+        <v>45412</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="5">
+        <v>45444</v>
+      </c>
+      <c r="C24" s="5">
+        <v>45504</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="5">
+        <v>45505</v>
+      </c>
+      <c r="C25" s="5">
+        <v>45596</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="5">
+        <v>45292</v>
+      </c>
+      <c r="C26" s="5">
+        <v>45351</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>